<commit_message>
larger axis and summary to submit
</commit_message>
<xml_diff>
--- a/results/summary_all.xlsx
+++ b/results/summary_all.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kauane Bordin\Meu Drive (kauanembordin@gmail.com)\Capítulo Functional Traits\plant_functional_traits_chapter\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D6E533-1D8C-4232-A017-3F338D64AE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10459EB-4398-46D3-A3A5-8445E7411178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{7345C443-23AC-41F1-AD75-3C55830770F6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="81">
   <si>
     <t>Trait</t>
   </si>
@@ -277,6 +277,12 @@
   <si>
     <t>14 (18%)</t>
   </si>
+  <si>
+    <t>Functional diversity</t>
+  </si>
+  <si>
+    <t>Functional dominance</t>
+  </si>
 </sst>
 </file>
 
@@ -374,9 +380,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -392,6 +395,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,72 +416,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagem 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18E180A-20BA-7CE6-EE8B-05FE880CA27D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7264400" y="0"/>
-          <a:ext cx="6661150" cy="3359150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -801,41 +741,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -6492,27 +6432,27 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection sqref="A1:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="6.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="18"/>
+      <c r="A1" s="17"/>
       <c r="B1" s="19" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -6520,7 +6460,7 @@
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="19" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
@@ -6529,863 +6469,863 @@
       <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="14" t="s">
+      <c r="C3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="16" t="s">
+      <c r="F3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="16" t="s">
+      <c r="K3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="16" t="s">
+      <c r="G4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="16" t="s">
+      <c r="H5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="14" t="s">
+      <c r="I6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="15" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="14" t="s">
+      <c r="J11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="11" t="s">
+      <c r="B14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="M14" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="15" t="s">
+      <c r="E15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="11" t="s">
+      <c r="G15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="14" t="s">
+      <c r="J15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="M15" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="13" t="s">
+      <c r="C18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" s="16" t="s">
+      <c r="G18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M18" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="14" t="s">
+      <c r="C19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="13" t="s">
+      <c r="I19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L19" s="15" t="s">
+      <c r="K19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J20" s="13" t="s">
+      <c r="I20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M20" s="16" t="s">
+      <c r="M20" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="11" t="s">
+      <c r="G21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L21" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="M21" s="16" t="s">
+      <c r="L21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M21" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="B22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="12" t="s">
+      <c r="G22" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="L22" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="M22" s="16" t="s">
+      <c r="M22" s="15" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7396,7 +7336,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
minor corrections to release
</commit_message>
<xml_diff>
--- a/results/summary_all.xlsx
+++ b/results/summary_all.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kauane Bordin\Meu Drive (kauanembordin@gmail.com)\Capítulo Functional Traits\plant_functional_traits_chapter\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10459EB-4398-46D3-A3A5-8445E7411178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B9D207-B93D-4F19-A696-F93A68875A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{7345C443-23AC-41F1-AD75-3C55830770F6}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
     <sheet name="rounded" sheetId="2" r:id="rId2"/>
-    <sheet name="to gt (2)" sheetId="4" r:id="rId3"/>
-    <sheet name="to gt" sheetId="3" r:id="rId4"/>
+    <sheet name="table 2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="81">
   <si>
     <t>Trait</t>
   </si>
@@ -419,9 +418,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -459,7 +458,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -565,7 +564,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -707,7 +706,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3742,7 +3741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A585B6B-0BC8-4131-AADC-335DF40288C6}">
   <dimension ref="A1:AM24"/>
   <sheetViews>
-    <sheetView topLeftCell="Y5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB3" sqref="AB3:AM22"/>
     </sheetView>
   </sheetViews>
@@ -7337,921 +7336,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25BE048-6E20-42BC-9E3C-2A8E40B44249}">
-  <dimension ref="A1:M22"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" t="s">
-        <v>56</v>
-      </c>
-      <c r="M12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" t="s">
-        <v>58</v>
-      </c>
-      <c r="L13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" t="s">
-        <v>61</v>
-      </c>
-      <c r="L14" t="s">
-        <v>46</v>
-      </c>
-      <c r="M14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K18" t="s">
-        <v>31</v>
-      </c>
-      <c r="L18" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" t="s">
-        <v>31</v>
-      </c>
-      <c r="L19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" t="s">
-        <v>31</v>
-      </c>
-      <c r="J20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" t="s">
-        <v>31</v>
-      </c>
-      <c r="M21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" t="s">
-        <v>69</v>
-      </c>
-      <c r="J22" t="s">
-        <v>70</v>
-      </c>
-      <c r="K22" t="s">
-        <v>67</v>
-      </c>
-      <c r="L22" t="s">
-        <v>69</v>
-      </c>
-      <c r="M22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>